<commit_message>
Update: Three Body Tech Heavier7Strings
</commit_message>
<xml_diff>
--- a/Three Body Technology/Heavier7Strings/xlsx/Heavier7Strings.xlsx
+++ b/Three Body Technology/Heavier7Strings/xlsx/Heavier7Strings.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="21555" windowHeight="10530"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="21555" windowHeight="10530" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Heavier7Strings(Main)" sheetId="9" r:id="rId1"/>
     <sheet name="Heavier7Strings(Harmonic)" sheetId="10" r:id="rId2"/>
     <sheet name="Heavier7Strings(FX)" sheetId="11" r:id="rId3"/>
-    <sheet name="DO NOT MODIFY!" sheetId="5" r:id="rId4"/>
+    <sheet name="Heavier7Strings(Stop)" sheetId="12" r:id="rId4"/>
+    <sheet name="Heavier7Strings(Muting CC1)" sheetId="13" r:id="rId5"/>
+    <sheet name="Heavier7Strings(Picking CC40)" sheetId="14" r:id="rId6"/>
+    <sheet name="DO NOT MODIFY!" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -91,8 +94,83 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>作成者</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>0=Default Color</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>作成者</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>0=Default Color</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>作成者</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>0=Default Color</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="192">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1"/>
@@ -643,19 +721,56 @@
     <t>Nose and FX</t>
   </si>
   <si>
-    <t>Slide(CC) On</t>
+    <t>Stop (Vel:15)</t>
+  </si>
+  <si>
+    <t>Stop (Vel:31)</t>
+  </si>
+  <si>
+    <t>Stop (Vel:47)</t>
+  </si>
+  <si>
+    <t>Stop (Vel:63)</t>
+  </si>
+  <si>
+    <t>Stop (Vel:79)</t>
+  </si>
+  <si>
+    <t>Stop (Vel:95)</t>
+  </si>
+  <si>
+    <t>Stop (Vel:111)</t>
+  </si>
+  <si>
+    <t>Stop (Vel:127)</t>
+  </si>
+  <si>
+    <t>Normal Play</t>
+  </si>
+  <si>
+    <t>Palm muting</t>
+  </si>
+  <si>
+    <t>Picking noise</t>
+  </si>
+  <si>
+    <t>Legato Slide(CC5)</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Slide(CC) Off</t>
+    <t>Legato Slide(CC5)</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Slide(CC) On</t>
+    <t>Auto</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Slide(CC) Off</t>
+    <t>Down Picking</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Up Picking</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1182,9 +1297,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1253,8 +1368,12 @@
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="H2" s="6">
+        <v>5</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10">
@@ -1279,8 +1398,12 @@
       <c r="G3" s="6">
         <v>120</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="H3" s="6">
+        <v>5</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10">
@@ -1305,8 +1428,12 @@
       <c r="G4" s="6">
         <v>120</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="H4" s="6">
+        <v>5</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10">
@@ -1331,8 +1458,12 @@
       <c r="G5" s="6">
         <v>120</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="H5" s="6">
+        <v>5</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10">
@@ -1357,19 +1488,23 @@
       <c r="G6" s="6">
         <v>120</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="H6" s="6">
+        <v>5</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="B7" s="6">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>11</v>
@@ -1388,29 +1523,15 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B8" s="6">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="2"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="6">
-        <v>5</v>
-      </c>
-      <c r="I8" s="6">
-        <v>0</v>
-      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10">
@@ -2385,29 +2506,17 @@
       <c r="I89" s="6"/>
       <c r="J89" s="3"/>
     </row>
-    <row r="90" spans="1:10">
-      <c r="A90" s="3"/>
-      <c r="B90" s="6"/>
-      <c r="C90" s="18"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="6"/>
-      <c r="F90" s="2"/>
-      <c r="G90" s="6"/>
-      <c r="H90" s="6"/>
-      <c r="I90" s="6"/>
-      <c r="J90" s="3"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B90">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B89">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H2:I90">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H2:I89">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty" sqref="G2:G90">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty" sqref="G2:G89">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
@@ -2422,19 +2531,19 @@
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$130</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F90</xm:sqref>
+          <xm:sqref>F2:F89</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D90</xm:sqref>
+          <xm:sqref>D2:D89</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E90</xm:sqref>
+          <xm:sqref>E2:E89</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5689,6 +5798,4160 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J103"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="35.625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="5.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="4" customWidth="1"/>
+    <col min="7" max="9" width="9.5" style="4" customWidth="1"/>
+    <col min="10" max="10" width="50.625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="6">
+        <v>15</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="6">
+        <v>31</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="6">
+        <v>47</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="6">
+        <v>63</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="6">
+        <v>79</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="6">
+        <v>95</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="6">
+        <v>111</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="6">
+        <v>127</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="3"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="3"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="3"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="3"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="3"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="3"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="3"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="3"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="3"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="3"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="3"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="3"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="3"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="3"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="3"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="3"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="3"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="3"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="3"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="3"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="3"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="3"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="3"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="3"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="3"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="3"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="3"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="3"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="3"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="3"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="3"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="3"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="3"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="3"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="3"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="3"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="3"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="3"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="3"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="3"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="3"/>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="3"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="3"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="3"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="3"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="3"/>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="3"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="3"/>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="3"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="3"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="3"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="3"/>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="3"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="3"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="3"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="3"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="3"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="3"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="3"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="3"/>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="3"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="3"/>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="3"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="3"/>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="3"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="3"/>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="3"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="3"/>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="3"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="3"/>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="3"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="3"/>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="3"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="3"/>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="3"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="3"/>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="3"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="3"/>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="3"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="3"/>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="3"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="3"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="3"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="3"/>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="3"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="3"/>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="3"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="3"/>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="3"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="3"/>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="3"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="3"/>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="3"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="3"/>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="3"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="3"/>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="3"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="3"/>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="3"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="3"/>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="3"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="3"/>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="3"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="3"/>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="3"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="3"/>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="3"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="3"/>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="3"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="3"/>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="3"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="3"/>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" s="3"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="3"/>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" s="3"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+      <c r="J89" s="3"/>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="3"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+      <c r="J90" s="3"/>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="3"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="3"/>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="3"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="3"/>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="3"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="3"/>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" s="3"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="18"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="3"/>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="3"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="3"/>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" s="3"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="3"/>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="3"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="3"/>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="3"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="3"/>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="3"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="18"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="3"/>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="3"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="18"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="3"/>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="3"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="18"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="3"/>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="3"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="3"/>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="3"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B103">
+      <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H2:I103">
+      <formula1>0</formula1>
+      <formula2>127</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty" sqref="G2:G103">
+      <formula1>0</formula1>
+      <formula2>127</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Choose from Drop-down list" prompt="If don’t use MIDI Note, set Cell value empty">
+          <x14:formula1>
+            <xm:f>'DO NOT MODIFY!'!$A$2:$A$130</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F103</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D103</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E103</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J102"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="35.625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="5.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="4" customWidth="1"/>
+    <col min="7" max="9" width="9.5" style="4" customWidth="1"/>
+    <col min="10" max="10" width="50.625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6">
+        <v>38</v>
+      </c>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6">
+        <v>80</v>
+      </c>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="3"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="3"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="3"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="3"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="3"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="3"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="3"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="3"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="3"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="3"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="3"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="3"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="3"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="3"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="3"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="3"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="3"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="3"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="3"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="3"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="3"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="3"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="3"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="3"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="3"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="3"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="3"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="3"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="3"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="3"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="3"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="3"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="3"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="3"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="3"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="3"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="3"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="3"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="3"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="3"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="3"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="3"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="3"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="3"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="3"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="3"/>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="3"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="3"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="3"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="3"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="3"/>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="3"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="3"/>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="3"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="3"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="3"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="3"/>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="3"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="3"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="3"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="3"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="3"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="3"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="3"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="3"/>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="3"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="3"/>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="3"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="3"/>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="3"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="3"/>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="3"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="3"/>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="3"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="3"/>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="3"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="3"/>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="3"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="3"/>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="3"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="3"/>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="3"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="3"/>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="3"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="3"/>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="3"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="3"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="3"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="3"/>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="3"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="3"/>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="3"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="3"/>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="3"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="3"/>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="3"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="3"/>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="3"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="3"/>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="3"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="3"/>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="3"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="3"/>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="3"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="3"/>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="3"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="3"/>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="3"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="3"/>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="3"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="3"/>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="3"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="3"/>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="3"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="3"/>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="3"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="3"/>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" s="3"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="3"/>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" s="3"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+      <c r="J89" s="3"/>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="3"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+      <c r="J90" s="3"/>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="3"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="3"/>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="3"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="3"/>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="3"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="3"/>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" s="3"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="18"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="3"/>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="3"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="3"/>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" s="3"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="3"/>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="3"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="3"/>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="3"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="3"/>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="3"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="18"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="3"/>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="3"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="18"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="3"/>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="3"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="18"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="3"/>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="3"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <dataValidations count="3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty" sqref="G2:G102">
+      <formula1>0</formula1>
+      <formula2>127</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H2:I102">
+      <formula1>0</formula1>
+      <formula2>127</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B102">
+      <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E102</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D102</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Choose from Drop-down list" prompt="If don’t use MIDI Note, set Cell value empty">
+          <x14:formula1>
+            <xm:f>'DO NOT MODIFY!'!$A$2:$A$130</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F102</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J102"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="35.625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="5.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="4" customWidth="1"/>
+    <col min="7" max="9" width="9.5" style="4" customWidth="1"/>
+    <col min="10" max="10" width="50.625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6">
+        <v>40</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6">
+        <v>40</v>
+      </c>
+      <c r="I3" s="6">
+        <v>22</v>
+      </c>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6">
+        <v>40</v>
+      </c>
+      <c r="I4" s="6">
+        <v>24</v>
+      </c>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="3"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="3"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="3"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="3"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="3"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="3"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="3"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="3"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="3"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="3"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="3"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="3"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="3"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="3"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="3"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="3"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="3"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="3"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="3"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="3"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="3"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="3"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="3"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="3"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="3"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="3"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="3"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="3"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="3"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="3"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="3"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="3"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="3"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="3"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="3"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="3"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="3"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="3"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="3"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="3"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="3"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="3"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="3"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="3"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="3"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="3"/>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="3"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="3"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="3"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="3"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="3"/>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="3"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="3"/>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="3"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="3"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="3"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="3"/>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="3"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="3"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="3"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="3"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="3"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="3"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="3"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="3"/>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="3"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="3"/>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="3"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="3"/>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="3"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="3"/>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="3"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="3"/>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="3"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="3"/>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="3"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="3"/>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="3"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="3"/>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="3"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="3"/>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="3"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="3"/>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="3"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="3"/>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="3"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="3"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="3"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="3"/>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="3"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="3"/>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="3"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="3"/>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="3"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="3"/>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="3"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="3"/>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="3"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="3"/>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="3"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="3"/>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="3"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="3"/>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="3"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="3"/>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="3"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="3"/>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="3"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="3"/>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="3"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="3"/>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="3"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="3"/>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="3"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="3"/>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="3"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="3"/>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" s="3"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="3"/>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" s="3"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+      <c r="J89" s="3"/>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="3"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+      <c r="J90" s="3"/>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="3"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="3"/>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="3"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="3"/>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="3"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="3"/>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" s="3"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="18"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="3"/>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="3"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="3"/>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" s="3"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="3"/>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="3"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="3"/>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="3"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="3"/>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="3"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="18"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="3"/>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="3"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="18"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="3"/>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="3"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="18"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="3"/>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="3"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B102">
+      <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H2:I102">
+      <formula1>0</formula1>
+      <formula2>127</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty" sqref="G2:G102">
+      <formula1>0</formula1>
+      <formula2>127</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Choose from Drop-down list" prompt="If don’t use MIDI Note, set Cell value empty">
+          <x14:formula1>
+            <xm:f>'DO NOT MODIFY!'!$A$2:$A$130</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F102</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D102</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E102</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>

</xml_diff>

<commit_message>
Modified: Heavier7Strings "Stop key-switch" data according to "SleepFreaks" article.
</commit_message>
<xml_diff>
--- a/Three Body Technology/Heavier7Strings/xlsx/Heavier7Strings.xlsx
+++ b/Three Body Technology/Heavier7Strings/xlsx/Heavier7Strings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="28830" windowHeight="6660" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="28830" windowHeight="6660" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Heavier7Strings(Main)" sheetId="1" r:id="rId1"/>
@@ -186,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="199">
   <si>
     <t>Name</t>
   </si>
@@ -696,30 +696,6 @@
   </si>
   <si>
     <t>Nose and FX</t>
-  </si>
-  <si>
-    <t>Stop (Vel:15)</t>
-  </si>
-  <si>
-    <t>Stop (Vel:31)</t>
-  </si>
-  <si>
-    <t>Stop (Vel:47)</t>
-  </si>
-  <si>
-    <t>Stop (Vel:63)</t>
-  </si>
-  <si>
-    <t>Stop (Vel:79)</t>
-  </si>
-  <si>
-    <t>Stop (Vel:95)</t>
-  </si>
-  <si>
-    <t>Stop (Vel:111)</t>
-  </si>
-  <si>
-    <t>Stop (Vel:127)</t>
   </si>
   <si>
     <t>Normal Play</t>
@@ -800,6 +776,15 @@
   <si>
     <t>Inspiration 1</t>
     <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Stop (Slide)</t>
+  </si>
+  <si>
+    <t>Stop (Left Hand)</t>
+  </si>
+  <si>
+    <t>Stop (Right Hand)</t>
   </si>
 </sst>
 </file>
@@ -1419,7 +1404,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1430,7 +1415,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K128"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75"/>
   <cols>
@@ -1655,13 +1640,13 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B8" s="12">
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>12</v>
@@ -1682,13 +1667,13 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B9" s="12">
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>12</v>
@@ -1709,13 +1694,13 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B10" s="12">
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>12</v>
@@ -1736,13 +1721,13 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B11" s="12">
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>12</v>
@@ -1763,13 +1748,13 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B12" s="12">
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>12</v>
@@ -1790,13 +1775,13 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="B13" s="12">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>12</v>
@@ -1817,13 +1802,13 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B14" s="12">
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>12</v>
@@ -1844,13 +1829,13 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B15" s="12">
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>12</v>
@@ -1871,13 +1856,13 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B16" s="12">
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>12</v>
@@ -1898,13 +1883,13 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B17" s="12">
         <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>12</v>
@@ -1925,13 +1910,13 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B18" s="12">
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>12</v>
@@ -1952,13 +1937,13 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B19" s="12">
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>12</v>
@@ -1979,13 +1964,13 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B20" s="12">
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>12</v>
@@ -2006,13 +1991,13 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B21" s="12">
         <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>12</v>
@@ -2033,13 +2018,13 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B22" s="12">
         <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>12</v>
@@ -2060,13 +2045,13 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B23" s="12">
         <v>2</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>12</v>
@@ -2087,13 +2072,13 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="1" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B24" s="12">
         <v>2</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>12</v>
@@ -2114,13 +2099,13 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B25" s="12">
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>12</v>
@@ -2141,13 +2126,13 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B26" s="12">
         <v>2</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>12</v>
@@ -7689,7 +7674,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75"/>
   <cols>
@@ -7752,7 +7737,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
@@ -7763,25 +7748,25 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>47</v>
       </c>
       <c r="G3" s="12">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -7790,25 +7775,25 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>47</v>
       </c>
       <c r="G4" s="12">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -7817,25 +7802,25 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>47</v>
       </c>
       <c r="G5" s="12">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -7843,135 +7828,65 @@
       <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" s="12">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="12">
-        <v>1</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="12">
-        <v>63</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B7" s="12">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="12">
-        <v>1</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="12">
-        <v>79</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" s="12">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="12">
-        <v>1</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="12">
-        <v>95</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B9" s="12">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="12">
-        <v>1</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="12">
-        <v>111</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B10" s="12">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="12">
-        <v>1</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="12">
-        <v>127</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -9666,13 +9581,13 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>12</v>
@@ -9693,13 +9608,13 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>12</v>
@@ -9720,13 +9635,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>12</v>
@@ -11499,13 +11414,13 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>12</v>
@@ -11526,13 +11441,13 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>12</v>
@@ -11553,13 +11468,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
FIXES: H7S - Stop
</commit_message>
<xml_diff>
--- a/Three Body Technology/Heavier7Strings/xlsx/Heavier7Strings.xlsx
+++ b/Three Body Technology/Heavier7Strings/xlsx/Heavier7Strings.xlsx
@@ -1134,10 +1134,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1534,7 +1534,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1560,13 +1560,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="20"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
@@ -3703,13 +3703,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="C1" s="20"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
@@ -5800,13 +5800,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="20"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
@@ -7855,13 +7855,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="20"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
@@ -7912,7 +7912,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -7935,7 +7935,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>47</v>
@@ -7962,7 +7962,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>47</v>
@@ -7989,7 +7989,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>47</v>
@@ -9700,13 +9700,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="C1" s="20"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
@@ -11545,13 +11545,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="20"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">

</xml_diff>

<commit_message>
Modifed: Heavier7Strings, Added: 8dio Century Harps
</commit_message>
<xml_diff>
--- a/Three Body Technology/Heavier7Strings/xlsx/Heavier7Strings.xlsx
+++ b/Three Body Technology/Heavier7Strings/xlsx/Heavier7Strings.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E25C3DB-D9EC-4871-AF51-A868729861A3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="28830" windowHeight="6660" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="28830" windowHeight="6660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Heavier7Strings(Main)" sheetId="1" r:id="rId1"/>
@@ -36,12 +37,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -76,12 +77,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -96,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -116,12 +117,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -136,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -156,12 +157,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -176,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -196,12 +197,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -216,7 +217,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -236,12 +237,12 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -256,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -719,9 +720,6 @@
     <t>Tapping</t>
   </si>
   <si>
-    <t>Legato Slide(CC5)</t>
-  </si>
-  <si>
     <t>N Harmonic @F12 Str1</t>
   </si>
   <si>
@@ -896,12 +894,16 @@
   </si>
   <si>
     <t>Heavier7Strings(Picking CC40)</t>
+  </si>
+  <si>
+    <t>Slide(CC5) On</t>
+    <phoneticPr fontId="5"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -1073,7 +1075,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1135,6 +1137,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1219,6 +1224,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1240,7 +1248,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1534,14 +1548,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K130"/>
   <sheetViews>
@@ -1561,12 +1575,12 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1">
       <c r="A1" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="C1" s="21"/>
+      <c r="C1" s="22"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
@@ -1621,8 +1635,12 @@
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="H4" s="12">
+        <v>5</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0</v>
+      </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
     </row>
@@ -1752,15 +1770,15 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
-        <v>147</v>
+        <v>205</v>
       </c>
       <c r="B9" s="12">
         <v>1</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D9" s="13" t="s">
+      <c r="C9" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="12">
@@ -1779,13 +1797,13 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B10" s="12">
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>12</v>
@@ -1806,13 +1824,13 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B11" s="12">
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>12</v>
@@ -1833,13 +1851,13 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B12" s="12">
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>12</v>
@@ -1860,13 +1878,13 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B13" s="12">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>12</v>
@@ -1887,13 +1905,13 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B14" s="12">
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>12</v>
@@ -1914,13 +1932,13 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B15" s="12">
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>12</v>
@@ -1941,13 +1959,13 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B16" s="12">
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>12</v>
@@ -1968,13 +1986,13 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B17" s="12">
         <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>12</v>
@@ -1995,13 +2013,13 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B18" s="12">
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>12</v>
@@ -2022,13 +2040,13 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B19" s="12">
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>12</v>
@@ -2049,13 +2067,13 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B20" s="12">
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>12</v>
@@ -2076,13 +2094,13 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B21" s="12">
         <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>12</v>
@@ -2103,13 +2121,13 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B22" s="12">
         <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>12</v>
@@ -2130,13 +2148,13 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B23" s="12">
         <v>2</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>12</v>
@@ -2157,13 +2175,13 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B24" s="12">
         <v>2</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>12</v>
@@ -2184,13 +2202,13 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B25" s="12">
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>12</v>
@@ -2211,13 +2229,13 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B26" s="12">
         <v>2</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>12</v>
@@ -2238,13 +2256,13 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B27" s="12">
         <v>2</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>12</v>
@@ -2265,13 +2283,13 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B28" s="12">
         <v>2</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>12</v>
@@ -3622,23 +3640,23 @@
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B130">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B130" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I130">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I130" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G130">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G130" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J130">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J130" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K130">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K130" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
@@ -3650,7 +3668,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -3659,7 +3677,7 @@
           </x14:formula2>
           <xm:sqref>D4:D130</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -3668,7 +3686,7 @@
           </x14:formula2>
           <xm:sqref>E4:E130</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0000-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -3684,7 +3702,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:K131"/>
   <sheetViews>
@@ -3704,12 +3722,12 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1">
       <c r="A1" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="C1" s="21"/>
+        <v>198</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="22"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
@@ -3771,13 +3789,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>12</v>
@@ -3798,13 +3816,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6" s="12">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>12</v>
@@ -3825,13 +3843,13 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B7" s="12">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>12</v>
@@ -3852,13 +3870,13 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8" s="12">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>12</v>
@@ -3879,13 +3897,13 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" s="12">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>12</v>
@@ -3906,13 +3924,13 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B10" s="12">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>12</v>
@@ -3933,13 +3951,13 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B11" s="12">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>12</v>
@@ -3960,13 +3978,13 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B12" s="12">
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>12</v>
@@ -3987,13 +4005,13 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B13" s="12">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>12</v>
@@ -4014,13 +4032,13 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B14" s="12">
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>12</v>
@@ -4041,13 +4059,13 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B15" s="12">
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>12</v>
@@ -4068,13 +4086,13 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B16" s="12">
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>12</v>
@@ -4095,13 +4113,13 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B17" s="12">
         <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>12</v>
@@ -4122,13 +4140,13 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B18" s="12">
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>12</v>
@@ -4149,13 +4167,13 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B19" s="12">
         <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>12</v>
@@ -4176,13 +4194,13 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B20" s="12">
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>12</v>
@@ -4203,13 +4221,13 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B21" s="12">
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>12</v>
@@ -4230,13 +4248,13 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B22" s="12">
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>12</v>
@@ -4257,13 +4275,13 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B23" s="12">
         <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>12</v>
@@ -4284,13 +4302,13 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B24" s="12">
         <v>3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>12</v>
@@ -4311,13 +4329,13 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B25" s="12">
         <v>3</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>12</v>
@@ -5720,23 +5738,23 @@
   </mergeCells>
   <phoneticPr fontId="6"/>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5747,7 +5765,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -5756,7 +5774,7 @@
           </x14:formula2>
           <xm:sqref>F4:F131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -5765,7 +5783,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -5781,7 +5799,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K131"/>
   <sheetViews>
@@ -5801,12 +5819,12 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1">
       <c r="A1" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="C1" s="21"/>
+        <v>198</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" s="22"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
@@ -5868,13 +5886,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>12</v>
@@ -5895,13 +5913,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6" s="12">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>12</v>
@@ -5922,13 +5940,13 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="12">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>12</v>
@@ -5949,13 +5967,13 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" s="12">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>12</v>
@@ -5976,13 +5994,13 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="12">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>12</v>
@@ -6003,13 +6021,13 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B10" s="12">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>12</v>
@@ -6030,13 +6048,13 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B11" s="12">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>12</v>
@@ -6057,13 +6075,13 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B12" s="12">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>12</v>
@@ -6084,13 +6102,13 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B13" s="12">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>12</v>
@@ -6111,13 +6129,13 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B14" s="12">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>12</v>
@@ -6138,13 +6156,13 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B15" s="12">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>12</v>
@@ -6165,13 +6183,13 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B16" s="12">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>12</v>
@@ -6192,13 +6210,13 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B17" s="12">
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>12</v>
@@ -6219,13 +6237,13 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B18" s="12">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>12</v>
@@ -6246,13 +6264,13 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B19" s="12">
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>12</v>
@@ -6273,13 +6291,13 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B20" s="12">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>12</v>
@@ -6300,13 +6318,13 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B21" s="12">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>12</v>
@@ -6327,13 +6345,13 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B22" s="12">
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>12</v>
@@ -7775,23 +7793,23 @@
   </mergeCells>
   <phoneticPr fontId="6"/>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7802,7 +7820,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0200-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -7811,7 +7829,7 @@
           </x14:formula2>
           <xm:sqref>F4:F131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -7820,7 +7838,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -7836,7 +7854,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K131"/>
   <sheetViews>
@@ -7856,12 +7874,12 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1">
       <c r="A1" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="C1" s="21"/>
+        <v>198</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" s="22"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
@@ -7923,13 +7941,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>12</v>
@@ -7950,13 +7968,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B6" s="12">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>12</v>
@@ -7977,13 +7995,13 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B7" s="12">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>12</v>
@@ -9620,23 +9638,23 @@
   </mergeCells>
   <phoneticPr fontId="6"/>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0300-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0300-000004000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9647,7 +9665,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0300-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -9656,7 +9674,7 @@
           </x14:formula2>
           <xm:sqref>F4:F131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -9665,7 +9683,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -9681,7 +9699,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K131"/>
   <sheetViews>
@@ -9701,12 +9719,12 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1">
       <c r="A1" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="C1" s="21"/>
+        <v>198</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" s="22"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
@@ -9768,13 +9786,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>12</v>
@@ -9795,13 +9813,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B6" s="12">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>12</v>
@@ -9822,13 +9840,13 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B7" s="12">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>12</v>
@@ -11465,23 +11483,23 @@
   </mergeCells>
   <phoneticPr fontId="6"/>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0400-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0400-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0400-000004000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -11492,7 +11510,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0400-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -11501,7 +11519,7 @@
           </x14:formula2>
           <xm:sqref>F4:F131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -11510,7 +11528,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -11526,7 +11544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K131"/>
   <sheetViews>
@@ -11546,12 +11564,12 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1">
       <c r="A1" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="C1" s="21"/>
+        <v>198</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" s="22"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
@@ -11613,13 +11631,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>12</v>
@@ -11640,13 +11658,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B6" s="12">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>12</v>
@@ -11667,13 +11685,13 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B7" s="12">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>12</v>
@@ -13310,23 +13328,23 @@
   </mergeCells>
   <phoneticPr fontId="6"/>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0500-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0500-000004000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -13337,7 +13355,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0500-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -13346,7 +13364,7 @@
           </x14:formula2>
           <xm:sqref>F4:F131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -13355,7 +13373,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -13371,8 +13389,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet4">
     <tabColor rgb="FF000000"/>
   </sheetPr>
   <dimension ref="A1:C258"/>

</xml_diff>